<commit_message>
bug fixes in api business
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestData_Api.xlsx
+++ b/Web/coyni/resources/TestData_Api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638A9198-CB62-4DD9-9A2E-DF777C3130E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098715F4-657E-405C-865F-45957FF00DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="10455" windowHeight="9180" firstSheet="8" activeTab="9" xr2:uid="{CB8AE841-AFC2-4DEA-A837-AD06A354DD94}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="10455" windowHeight="9180" firstSheet="8" activeTab="10" xr2:uid="{CB8AE841-AFC2-4DEA-A837-AD06A354DD94}"/>
   </bookViews>
   <sheets>
     <sheet name="IdentityVerification" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4939" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4950" uniqueCount="1026">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2394,9 +2394,6 @@
     <t>Delete External Bank Account</t>
   </si>
   <si>
-    <t>3456</t>
-  </si>
-  <si>
     <t>testBusinessSettingsDeleteDebitCard</t>
   </si>
   <si>
@@ -3170,6 +3167,21 @@
   </si>
   <si>
     <t>1.00</t>
+  </si>
+  <si>
+    <t>withdrawsignetAccountHeading</t>
+  </si>
+  <si>
+    <t>4429 5497 8723 7693</t>
+  </si>
+  <si>
+    <t>122105278</t>
+  </si>
+  <si>
+    <t>0000000016</t>
+  </si>
+  <si>
+    <t>0016</t>
   </si>
 </sst>
 </file>
@@ -8828,7 +8840,7 @@
       <c r="BE39" s="4"/>
       <c r="BF39" s="4"/>
     </row>
-    <row r="40" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>198</v>
       </c>
@@ -8944,7 +8956,7 @@
       <c r="BE40" s="4"/>
       <c r="BF40" s="4"/>
     </row>
-    <row r="41" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>199</v>
       </c>
@@ -9067,7 +9079,7 @@
       <c r="BF41" s="4"/>
       <c r="BG41" s="4"/>
     </row>
-    <row r="42" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>217</v>
       </c>
@@ -9168,7 +9180,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>226</v>
       </c>
@@ -9273,7 +9285,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>226</v>
       </c>
@@ -9378,7 +9390,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>226</v>
       </c>
@@ -9481,7 +9493,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="46" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>226</v>
       </c>
@@ -9584,7 +9596,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="47" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>226</v>
       </c>
@@ -9687,7 +9699,7 @@
       </c>
       <c r="BO47" s="17"/>
     </row>
-    <row r="48" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>226</v>
       </c>
@@ -9792,7 +9804,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>226</v>
       </c>
@@ -9897,7 +9909,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="50" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>247</v>
       </c>
@@ -9998,7 +10010,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>248</v>
       </c>
@@ -10362,8 +10374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DD43B4-840D-4E6E-B5BD-15D06968843D}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10967,10 +10979,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C13BE43-F382-436A-BAAC-4675AC294583}">
-  <dimension ref="A1:AQ26"/>
+  <dimension ref="A1:AU26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11018,10 +11030,14 @@
     <col min="41" max="41" width="26" style="69" customWidth="1"/>
     <col min="42" max="42" width="18.7109375" style="69" customWidth="1"/>
     <col min="43" max="43" width="41.5703125" style="69" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="69"/>
+    <col min="44" max="44" width="14.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.42578125" style="69" customWidth="1"/>
+    <col min="47" max="47" width="22.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -11151,8 +11167,20 @@
       <c r="AQ1" s="67" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="2" spans="1:43" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AR1" s="69" t="s">
+        <v>741</v>
+      </c>
+      <c r="AS1" s="69" t="s">
+        <v>742</v>
+      </c>
+      <c r="AT1" s="69" t="s">
+        <v>743</v>
+      </c>
+      <c r="AU1" s="69" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="69" t="s">
         <v>754</v>
       </c>
@@ -11226,7 +11254,7 @@
       <c r="Y2" s="106"/>
       <c r="AB2" s="107"/>
     </row>
-    <row r="3" spans="1:43" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="69" t="s">
         <v>756</v>
       </c>
@@ -11298,7 +11326,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="69" t="s">
         <v>608</v>
       </c>
@@ -11341,8 +11369,20 @@
       <c r="AD4" s="69" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AR4" s="70" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AS4" s="70" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AT4" s="70" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AU4" s="70" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="69" t="s">
         <v>765</v>
       </c>
@@ -11380,18 +11420,18 @@
       <c r="AE5" s="109"/>
       <c r="AF5" s="79"/>
       <c r="AO5" s="70" t="s">
-        <v>767</v>
+        <v>1025</v>
       </c>
       <c r="AQ5" s="79" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
+        <v>767</v>
+      </c>
+      <c r="B6" s="69" t="s">
         <v>768</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>769</v>
       </c>
       <c r="C6" s="70" t="s">
         <v>68</v>
@@ -11433,12 +11473,12 @@
         <v>692</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
+        <v>769</v>
+      </c>
+      <c r="B7" s="69" t="s">
         <v>770</v>
-      </c>
-      <c r="B7" s="69" t="s">
-        <v>771</v>
       </c>
       <c r="C7" s="70" t="s">
         <v>68</v>
@@ -11505,12 +11545,12 @@
       </c>
       <c r="X7" s="70"/>
     </row>
-    <row r="8" spans="1:43" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
+        <v>771</v>
+      </c>
+      <c r="B8" s="69" t="s">
         <v>772</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>773</v>
       </c>
       <c r="C8" s="70" t="s">
         <v>68</v>
@@ -11540,28 +11580,28 @@
         <v>74</v>
       </c>
       <c r="L8" s="110" t="s">
+        <v>773</v>
+      </c>
+      <c r="M8" s="28" t="s">
         <v>774</v>
-      </c>
-      <c r="M8" s="28" t="s">
-        <v>775</v>
       </c>
       <c r="N8" s="75" t="s">
         <v>678</v>
       </c>
       <c r="O8" s="76" t="s">
+        <v>775</v>
+      </c>
+      <c r="P8" s="77" t="s">
         <v>776</v>
       </c>
-      <c r="P8" s="77" t="s">
+      <c r="Q8" s="69" t="s">
         <v>777</v>
-      </c>
-      <c r="Q8" s="69" t="s">
-        <v>778</v>
       </c>
       <c r="R8" s="69" t="s">
         <v>682</v>
       </c>
       <c r="S8" s="69" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="T8" s="70" t="s">
         <v>683</v>
@@ -11580,12 +11620,12 @@
         <v>702</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
+        <v>779</v>
+      </c>
+      <c r="B9" s="69" t="s">
         <v>780</v>
-      </c>
-      <c r="B9" s="69" t="s">
-        <v>781</v>
       </c>
       <c r="C9" s="70" t="s">
         <v>68</v>
@@ -11618,21 +11658,21 @@
         <v>177</v>
       </c>
       <c r="AJ9" s="69" t="s">
+        <v>781</v>
+      </c>
+      <c r="AK9" s="69" t="s">
         <v>782</v>
       </c>
-      <c r="AK9" s="69" t="s">
+      <c r="AL9" s="69" t="s">
         <v>783</v>
       </c>
-      <c r="AL9" s="69" t="s">
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="10" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
+      <c r="B10" s="111" t="s">
         <v>785</v>
-      </c>
-      <c r="B10" s="111" t="s">
-        <v>786</v>
       </c>
       <c r="C10" s="112" t="s">
         <v>68</v>
@@ -11667,15 +11707,15 @@
       </c>
       <c r="AL10" s="109"/>
       <c r="AM10" s="69" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11" s="69" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="B11" s="69" t="s">
         <v>788</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>789</v>
       </c>
       <c r="C11" s="112" t="s">
         <v>68</v>
@@ -11729,7 +11769,7 @@
         <v>202</v>
       </c>
       <c r="T11" s="70" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="U11" s="69" t="s">
         <v>205</v>
@@ -11744,12 +11784,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C12" s="112" t="s">
         <v>101</v>
@@ -11815,15 +11855,15 @@
         <v>600</v>
       </c>
       <c r="X12" s="124" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A13" s="69" t="s">
+        <v>787</v>
+      </c>
+      <c r="B13" s="69" t="s">
         <v>792</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
-        <v>788</v>
-      </c>
-      <c r="B13" s="69" t="s">
-        <v>793</v>
       </c>
       <c r="C13" s="112" t="s">
         <v>105</v>
@@ -11862,7 +11902,7 @@
         <v>697</v>
       </c>
       <c r="O13" s="69" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="P13" s="121" t="s">
         <v>699</v>
@@ -11889,15 +11929,15 @@
         <v>600</v>
       </c>
       <c r="X13" s="124" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C14" s="112" t="s">
         <v>108</v>
@@ -11930,7 +11970,7 @@
         <v>695</v>
       </c>
       <c r="M14" s="125" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="N14" s="75" t="s">
         <v>697</v>
@@ -11960,15 +12000,15 @@
         <v>600</v>
       </c>
       <c r="X14" s="126" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>787</v>
+      </c>
+      <c r="B15" s="69" t="s">
         <v>797</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
-        <v>788</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>798</v>
       </c>
       <c r="C15" s="112" t="s">
         <v>116</v>
@@ -12010,7 +12050,7 @@
         <v>698</v>
       </c>
       <c r="P15" s="70" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="Q15" s="123" t="s">
         <v>681</v>
@@ -12034,15 +12074,15 @@
         <v>600</v>
       </c>
       <c r="X15" s="126" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>787</v>
+      </c>
+      <c r="B16" s="69" t="s">
         <v>800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
-        <v>788</v>
-      </c>
-      <c r="B16" s="69" t="s">
-        <v>801</v>
       </c>
       <c r="C16" s="112" t="s">
         <v>148</v>
@@ -12087,7 +12127,7 @@
         <v>699</v>
       </c>
       <c r="Q16" s="127" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="R16" s="123" t="s">
         <v>682</v>
@@ -12109,15 +12149,15 @@
       </c>
       <c r="X16" s="126"/>
       <c r="AP16" s="69" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C17" s="112" t="s">
         <v>120</v>
@@ -12180,15 +12220,15 @@
         <v>600</v>
       </c>
       <c r="X17" s="119" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B18" s="69" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C18" s="112" t="s">
         <v>123</v>
@@ -12251,15 +12291,15 @@
         <v>600</v>
       </c>
       <c r="X18" s="126" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C19" s="112" t="s">
         <v>127</v>
@@ -12322,15 +12362,15 @@
         <v>600</v>
       </c>
       <c r="X19" s="126" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C20" s="112" t="s">
         <v>137</v>
@@ -12395,10 +12435,10 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C21" s="112" t="s">
         <v>141</v>
@@ -12456,15 +12496,15 @@
         <v>600</v>
       </c>
       <c r="X21" s="119" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C22" s="112" t="s">
         <v>145</v>
@@ -12521,15 +12561,15 @@
         <v>600</v>
       </c>
       <c r="X22" s="119" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C23" s="112" t="s">
         <v>132</v>
@@ -12597,10 +12637,10 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="69" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C24" s="112" t="s">
         <v>134</v>
@@ -12663,15 +12703,15 @@
         <v>600</v>
       </c>
       <c r="X24" s="119" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
+        <v>817</v>
+      </c>
+      <c r="B25" s="69" t="s">
         <v>818</v>
-      </c>
-      <c r="B25" s="69" t="s">
-        <v>819</v>
       </c>
       <c r="C25" s="112" t="s">
         <v>68</v>
@@ -12701,40 +12741,40 @@
         <v>74</v>
       </c>
       <c r="L25" s="69" t="s">
+        <v>819</v>
+      </c>
+      <c r="M25" s="69" t="s">
         <v>820</v>
       </c>
-      <c r="M25" s="69" t="s">
+      <c r="O25" s="69" t="s">
         <v>821</v>
       </c>
-      <c r="O25" s="69" t="s">
+      <c r="P25" s="69" t="s">
         <v>822</v>
       </c>
-      <c r="P25" s="69" t="s">
+      <c r="Q25" s="69" t="s">
         <v>823</v>
       </c>
-      <c r="Q25" s="69" t="s">
+      <c r="R25" s="69" t="s">
+        <v>823</v>
+      </c>
+      <c r="S25" s="69" t="s">
         <v>824</v>
       </c>
-      <c r="R25" s="69" t="s">
-        <v>824</v>
-      </c>
-      <c r="S25" s="69" t="s">
+      <c r="U25" s="69" t="s">
         <v>825</v>
       </c>
-      <c r="U25" s="69" t="s">
+      <c r="W25" s="112" t="s">
         <v>826</v>
-      </c>
-      <c r="W25" s="112" t="s">
-        <v>827</v>
       </c>
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
+        <v>827</v>
+      </c>
+      <c r="B26" s="69" t="s">
         <v>828</v>
-      </c>
-      <c r="B26" s="69" t="s">
-        <v>829</v>
       </c>
       <c r="C26" s="112" t="s">
         <v>68</v>
@@ -12776,7 +12816,7 @@
         <v>698</v>
       </c>
       <c r="P26" s="77" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="Q26" s="69" t="s">
         <v>681</v>
@@ -12797,7 +12837,7 @@
         <v>84</v>
       </c>
       <c r="W26" s="70" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="X26" s="70"/>
     </row>
@@ -12911,10 +12951,10 @@
         <v>50</v>
       </c>
       <c r="M1" s="82" t="s">
+        <v>831</v>
+      </c>
+      <c r="N1" s="82" t="s">
         <v>832</v>
-      </c>
-      <c r="N1" s="82" t="s">
-        <v>833</v>
       </c>
       <c r="O1" s="82" t="s">
         <v>54</v>
@@ -12926,10 +12966,10 @@
         <v>56</v>
       </c>
       <c r="R1" s="82" t="s">
+        <v>833</v>
+      </c>
+      <c r="S1" s="82" t="s">
         <v>834</v>
-      </c>
-      <c r="S1" s="82" t="s">
-        <v>835</v>
       </c>
       <c r="T1" s="82" t="s">
         <v>635</v>
@@ -12953,7 +12993,7 @@
         <v>24</v>
       </c>
       <c r="AA1" s="82" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="AB1" s="82" t="s">
         <v>545</v>
@@ -12961,10 +13001,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>837</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>838</v>
       </c>
       <c r="C2" s="84" t="s">
         <v>68</v>
@@ -12994,13 +13034,13 @@
         <v>74</v>
       </c>
       <c r="L2" s="88" t="s">
+        <v>838</v>
+      </c>
+      <c r="M2" s="88" t="s">
         <v>839</v>
       </c>
-      <c r="M2" s="88" t="s">
+      <c r="N2" s="88" t="s">
         <v>840</v>
-      </c>
-      <c r="N2" s="88" t="s">
-        <v>841</v>
       </c>
       <c r="O2" s="129" t="s">
         <v>610</v>
@@ -13021,18 +13061,18 @@
       <c r="Y2" s="41"/>
       <c r="Z2" s="41"/>
       <c r="AA2" s="36" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="AB2" s="84" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
+        <v>842</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>843</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>844</v>
       </c>
       <c r="C3" s="84" t="s">
         <v>68</v>
@@ -13062,13 +13102,13 @@
         <v>74</v>
       </c>
       <c r="L3" s="88" t="s">
+        <v>838</v>
+      </c>
+      <c r="M3" s="88" t="s">
         <v>839</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="N3" s="88" t="s">
         <v>840</v>
-      </c>
-      <c r="N3" s="88" t="s">
-        <v>841</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -13077,10 +13117,10 @@
         <v>760</v>
       </c>
       <c r="S3" s="41" t="s">
+        <v>844</v>
+      </c>
+      <c r="T3" s="41" t="s">
         <v>845</v>
-      </c>
-      <c r="T3" s="41" t="s">
-        <v>846</v>
       </c>
       <c r="U3" s="41" t="s">
         <v>681</v>
@@ -13092,19 +13132,19 @@
         <v>202</v>
       </c>
       <c r="X3" s="33" t="s">
+        <v>846</v>
+      </c>
+      <c r="Y3" s="84" t="s">
         <v>847</v>
-      </c>
-      <c r="Y3" s="84" t="s">
-        <v>848</v>
       </c>
       <c r="Z3" s="41" t="s">
         <v>84</v>
       </c>
       <c r="AA3" s="36" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="AB3" s="84" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -13182,7 +13222,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="135" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="M1" s="136" t="s">
         <v>630</v>
@@ -13200,12 +13240,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
+        <v>849</v>
+      </c>
+      <c r="B2" s="137" t="s">
         <v>850</v>
-      </c>
-      <c r="B2" s="137" t="s">
-        <v>851</v>
       </c>
       <c r="C2" s="138" t="s">
         <v>68</v>
@@ -13235,18 +13275,18 @@
         <v>74</v>
       </c>
       <c r="L2" s="142" t="s">
+        <v>851</v>
+      </c>
+      <c r="M2" s="55" t="s">
         <v>852</v>
       </c>
-      <c r="M2" s="55" t="s">
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="137" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="137" t="s">
+      <c r="B3" s="137" t="s">
         <v>854</v>
-      </c>
-      <c r="B3" s="137" t="s">
-        <v>855</v>
       </c>
       <c r="C3" s="138" t="s">
         <v>68</v>
@@ -13276,18 +13316,18 @@
         <v>74</v>
       </c>
       <c r="L3" s="142" t="s">
+        <v>851</v>
+      </c>
+      <c r="M3" s="55" t="s">
         <v>852</v>
       </c>
-      <c r="M3" s="55" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="137" t="s">
+        <v>855</v>
+      </c>
+      <c r="B4" s="137" t="s">
         <v>856</v>
-      </c>
-      <c r="B4" s="137" t="s">
-        <v>857</v>
       </c>
       <c r="C4" s="138" t="s">
         <v>68</v>
@@ -13317,27 +13357,27 @@
         <v>74</v>
       </c>
       <c r="L4" s="142" t="s">
+        <v>851</v>
+      </c>
+      <c r="M4" s="55" t="s">
         <v>852</v>
-      </c>
-      <c r="M4" s="55" t="s">
-        <v>853</v>
       </c>
       <c r="N4" s="137" t="s">
         <v>523</v>
       </c>
       <c r="O4" s="137" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="Q4" s="138" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="137" t="s">
+        <v>858</v>
+      </c>
+      <c r="B5" s="137" t="s">
         <v>859</v>
-      </c>
-      <c r="B5" s="137" t="s">
-        <v>860</v>
       </c>
       <c r="C5" s="138" t="s">
         <v>68</v>
@@ -13367,7 +13407,7 @@
         <v>74</v>
       </c>
       <c r="L5" s="142" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>
@@ -13462,10 +13502,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
+        <v>860</v>
+      </c>
+      <c r="B2" s="132" t="s">
         <v>861</v>
-      </c>
-      <c r="B2" s="132" t="s">
-        <v>862</v>
       </c>
       <c r="C2" s="146" t="s">
         <v>68</v>
@@ -13505,7 +13545,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B3" s="69" t="s">
         <v>509</v>
@@ -13549,7 +13589,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B4" s="69" t="s">
         <v>509</v>
@@ -13593,7 +13633,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B5" s="69" t="s">
         <v>510</v>
@@ -13637,7 +13677,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>512</v>
@@ -13681,7 +13721,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B7" s="69" t="s">
         <v>512</v>
@@ -13725,7 +13765,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B8" s="69" t="s">
         <v>512</v>
@@ -13769,7 +13809,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B9" s="69" t="s">
         <v>512</v>
@@ -13813,7 +13853,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>517</v>
@@ -13849,15 +13889,15 @@
         <v>273</v>
       </c>
       <c r="N10" s="149" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
+        <v>863</v>
+      </c>
+      <c r="B11" s="69" t="s">
         <v>864</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>865</v>
       </c>
       <c r="C11" s="146" t="s">
         <v>68</v>
@@ -13887,7 +13927,7 @@
         <v>74</v>
       </c>
       <c r="M11" s="69" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="N11" s="69" t="s">
         <v>121</v>
@@ -13898,10 +13938,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="69" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C12" s="146" t="s">
         <v>101</v>
@@ -13931,7 +13971,7 @@
         <v>74</v>
       </c>
       <c r="M12" s="69" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="N12" s="69" t="s">
         <v>121</v>
@@ -13942,10 +13982,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C13" s="146" t="s">
         <v>105</v>
@@ -13975,7 +14015,7 @@
         <v>74</v>
       </c>
       <c r="M13" s="69" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N13" s="69" t="s">
         <v>121</v>
@@ -13986,10 +14026,10 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="69" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C14" s="146" t="s">
         <v>108</v>
@@ -14019,7 +14059,7 @@
         <v>74</v>
       </c>
       <c r="M14" s="69" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="N14" s="69" t="s">
         <v>121</v>
@@ -14030,10 +14070,10 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="69" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C15" s="146" t="s">
         <v>116</v>
@@ -14190,18 +14230,18 @@
         <v>50</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>874</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
+        <v>875</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>876</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>877</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14238,13 +14278,13 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="11" t="s">
+        <v>877</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="4" t="s">
         <v>879</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>880</v>
       </c>
     </row>
   </sheetData>
@@ -14329,7 +14369,7 @@
         <v>50</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>41</v>
@@ -14338,16 +14378,16 @@
         <v>42</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>882</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>883</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>884</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>885</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>276</v>
@@ -14359,24 +14399,24 @@
         <v>11</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>886</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>887</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
+        <v>888</v>
+      </c>
+      <c r="B2" t="s">
         <v>889</v>
-      </c>
-      <c r="B2" t="s">
-        <v>890</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14406,15 +14446,15 @@
         <v>74</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>891</v>
+      </c>
+      <c r="B3" t="s">
         <v>892</v>
-      </c>
-      <c r="B3" t="s">
-        <v>893</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>68</v>
@@ -14444,51 +14484,51 @@
         <v>74</v>
       </c>
       <c r="M3" s="11" t="s">
+        <v>893</v>
+      </c>
+      <c r="N3" t="s">
         <v>894</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>895</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" s="6" t="s">
         <v>896</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="17" t="s">
         <v>897</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="R3" s="131" t="s">
         <v>898</v>
       </c>
-      <c r="R3" s="131" t="s">
+      <c r="S3" s="153" t="s">
         <v>899</v>
       </c>
-      <c r="S3" s="153" t="s">
-        <v>900</v>
-      </c>
       <c r="T3" s="153" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="U3" t="s">
         <v>523</v>
       </c>
       <c r="V3" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="W3" t="s">
         <v>901</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" t="s">
         <v>903</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>904</v>
+      </c>
+      <c r="B4" t="s">
         <v>905</v>
-      </c>
-      <c r="B4" t="s">
-        <v>906</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>68</v>
@@ -14521,10 +14561,10 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>906</v>
+      </c>
+      <c r="B5" t="s">
         <v>907</v>
-      </c>
-      <c r="B5" t="s">
-        <v>908</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>68</v>
@@ -14559,10 +14599,10 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>101</v>
@@ -14592,15 +14632,15 @@
         <v>74</v>
       </c>
       <c r="X6" s="155" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>105</v>
@@ -14630,15 +14670,15 @@
         <v>74</v>
       </c>
       <c r="X7" s="154" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>912</v>
+      </c>
+      <c r="B8" t="s">
         <v>913</v>
-      </c>
-      <c r="B8" t="s">
-        <v>914</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>68</v>
@@ -14670,10 +14710,10 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>914</v>
+      </c>
+      <c r="B9" t="s">
         <v>915</v>
-      </c>
-      <c r="B9" t="s">
-        <v>916</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>68</v>
@@ -14703,7 +14743,7 @@
         <v>74</v>
       </c>
       <c r="Y9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -14787,10 +14827,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>917</v>
+      </c>
+      <c r="B2" t="s">
         <v>918</v>
-      </c>
-      <c r="B2" t="s">
-        <v>919</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14820,7 +14860,7 @@
         <v>74</v>
       </c>
       <c r="L2" s="156" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -14910,10 +14950,10 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C2" s="143" t="s">
         <v>68</v>
@@ -14953,7 +14993,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B3" t="s">
         <v>509</v>
@@ -14997,7 +15037,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B4" t="s">
         <v>510</v>
@@ -15041,7 +15081,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B5" t="s">
         <v>512</v>
@@ -15085,7 +15125,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B6" t="s">
         <v>512</v>
@@ -15129,7 +15169,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B7" t="s">
         <v>512</v>
@@ -15173,7 +15213,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B8" t="s">
         <v>512</v>
@@ -15217,10 +15257,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B9" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C9" s="143" t="s">
         <v>127</v>
@@ -15250,7 +15290,7 @@
         <v>74</v>
       </c>
       <c r="M9" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="N9" t="s">
         <v>121</v>
@@ -15261,10 +15301,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B10" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C10" s="143" t="s">
         <v>132</v>
@@ -15294,7 +15334,7 @@
         <v>74</v>
       </c>
       <c r="M10" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N10" t="s">
         <v>121</v>
@@ -15305,10 +15345,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B11" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C11" s="143" t="s">
         <v>134</v>
@@ -15338,7 +15378,7 @@
         <v>74</v>
       </c>
       <c r="M11" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="N11" t="s">
         <v>121</v>
@@ -15347,12 +15387,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>921</v>
+      </c>
+      <c r="B12" t="s">
         <v>922</v>
-      </c>
-      <c r="B12" t="s">
-        <v>923</v>
       </c>
       <c r="C12" s="143" t="s">
         <v>68</v>
@@ -15471,21 +15511,21 @@
         <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>925</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>927</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>928</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -15512,16 +15552,16 @@
         <v>220</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>929</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>930</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>931</v>
       </c>
     </row>
   </sheetData>
@@ -16225,10 +16265,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B2" t="s">
         <v>932</v>
-      </c>
-      <c r="B2" t="s">
-        <v>933</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16258,15 +16298,15 @@
         <v>74</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>934</v>
+      </c>
+      <c r="B3" t="s">
         <v>935</v>
-      </c>
-      <c r="B3" t="s">
-        <v>936</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16296,15 +16336,15 @@
         <v>74</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B4" t="s">
         <v>937</v>
-      </c>
-      <c r="B4" t="s">
-        <v>938</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>68</v>
@@ -16334,7 +16374,7 @@
         <v>74</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
   </sheetData>
@@ -16412,15 +16452,15 @@
         <v>50</v>
       </c>
       <c r="M1" s="152" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B2" t="s">
         <v>940</v>
-      </c>
-      <c r="B2" t="s">
-        <v>941</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16450,10 +16490,10 @@
         <v>74</v>
       </c>
       <c r="L2" t="s">
+        <v>941</v>
+      </c>
+      <c r="M2" t="s">
         <v>942</v>
-      </c>
-      <c r="M2" t="s">
-        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -16529,10 +16569,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
+        <v>943</v>
+      </c>
+      <c r="B2" t="s">
         <v>944</v>
-      </c>
-      <c r="B2" t="s">
-        <v>945</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16562,15 +16602,15 @@
         <v>74</v>
       </c>
       <c r="L2" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
+        <v>946</v>
+      </c>
+      <c r="B3" t="s">
         <v>947</v>
-      </c>
-      <c r="B3" t="s">
-        <v>948</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16600,7 +16640,7 @@
         <v>74</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>
@@ -16680,13 +16720,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="152" t="s">
+        <v>948</v>
+      </c>
+      <c r="M1" s="152" t="s">
         <v>949</v>
       </c>
-      <c r="M1" s="152" t="s">
+      <c r="N1" s="152" t="s">
         <v>950</v>
-      </c>
-      <c r="N1" s="152" t="s">
-        <v>951</v>
       </c>
       <c r="O1" s="152" t="s">
         <v>636</v>
@@ -16704,15 +16744,15 @@
         <v>51</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
+        <v>952</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>953</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>954</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16742,30 +16782,30 @@
         <v>74</v>
       </c>
       <c r="L2" s="33" t="s">
+        <v>954</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>955</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>956</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="O2" s="7" t="s">
         <v>957</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>958</v>
       </c>
       <c r="P2" s="157"/>
       <c r="Q2" s="157"/>
       <c r="R2" s="157"/>
       <c r="T2" s="158" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
+        <v>959</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>960</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>961</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16795,25 +16835,25 @@
         <v>74</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="M3" s="157"/>
       <c r="N3" s="33"/>
       <c r="O3" s="157"/>
       <c r="P3" s="159" t="s">
+        <v>961</v>
+      </c>
+      <c r="Q3" s="159" t="s">
         <v>962</v>
-      </c>
-      <c r="Q3" s="159" t="s">
-        <v>963</v>
       </c>
       <c r="R3" s="157"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>68</v>
@@ -16845,22 +16885,22 @@
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
       <c r="N4" s="9" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="O4" s="157"/>
       <c r="P4" s="159"/>
       <c r="Q4" s="159"/>
       <c r="R4" s="157" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="S4" s="160"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="99" t="s">
+        <v>966</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>967</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>968</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>68</v>
@@ -16890,16 +16930,16 @@
         <v>74</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="M5" s="33" t="s">
+        <v>968</v>
+      </c>
+      <c r="N5" s="33" t="s">
         <v>969</v>
       </c>
-      <c r="N5" s="33" t="s">
-        <v>970</v>
-      </c>
       <c r="O5" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
   </sheetData>
@@ -16982,10 +17022,10 @@
         <v>50</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>971</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>972</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>477</v>
@@ -16996,10 +17036,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
+        <v>972</v>
+      </c>
+      <c r="B2" t="s">
         <v>973</v>
-      </c>
-      <c r="B2" t="s">
-        <v>974</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -17029,15 +17069,15 @@
         <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>975</v>
+      </c>
+      <c r="B3" t="s">
         <v>976</v>
-      </c>
-      <c r="B3" t="s">
-        <v>977</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>68</v>
@@ -17067,19 +17107,19 @@
         <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="M3" t="s">
+        <v>977</v>
+      </c>
+      <c r="N3" t="s">
         <v>978</v>
-      </c>
-      <c r="N3" t="s">
-        <v>979</v>
       </c>
       <c r="O3" t="s">
         <v>523</v>
       </c>
       <c r="P3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
   </sheetData>
@@ -17151,15 +17191,15 @@
         <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>981</v>
+      </c>
+      <c r="B2" t="s">
         <v>982</v>
-      </c>
-      <c r="B2" t="s">
-        <v>983</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>68</v>
@@ -17189,7 +17229,7 @@
         <v>74</v>
       </c>
       <c r="L2" s="48" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -17261,21 +17301,21 @@
         <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>985</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>986</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>988</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>989</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -17302,16 +17342,16 @@
         <v>220</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>989</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>991</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -17390,39 +17430,39 @@
         <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>993</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>994</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>995</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>526</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>996</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>997</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>998</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>999</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>1000</v>
       </c>
       <c r="C2" s="162" t="s">
         <v>68</v>
@@ -17452,15 +17492,15 @@
         <v>74</v>
       </c>
       <c r="S2" s="165" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>1002</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1003</v>
       </c>
       <c r="C3" s="162" t="s">
         <v>68</v>
@@ -17490,33 +17530,33 @@
         <v>74</v>
       </c>
       <c r="L3" s="20" t="s">
+        <v>1003</v>
+      </c>
+      <c r="M3" s="165" t="s">
         <v>1004</v>
-      </c>
-      <c r="M3" s="165" t="s">
-        <v>1005</v>
       </c>
       <c r="N3" s="165" t="s">
         <v>28</v>
       </c>
       <c r="O3" s="165" t="s">
+        <v>1005</v>
+      </c>
+      <c r="P3" s="165" t="s">
         <v>1006</v>
       </c>
-      <c r="P3" s="165" t="s">
+      <c r="Q3" s="20" t="s">
         <v>1007</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="R3" s="162" t="s">
         <v>1008</v>
-      </c>
-      <c r="R3" s="162" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B4" t="s">
         <v>1010</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1011</v>
       </c>
       <c r="C4" s="162" t="s">
         <v>68</v>
@@ -17546,7 +17586,7 @@
         <v>74</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
   </sheetData>
@@ -18816,7 +18856,7 @@
       <c r="Q11" s="33"/>
       <c r="R11" s="33"/>
       <c r="S11" s="45" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="T11" s="33" t="s">
         <v>91</v>
@@ -18827,7 +18867,7 @@
       <c r="V11" s="41"/>
       <c r="W11" s="41"/>
       <c r="X11" s="45" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -19194,7 +19234,7 @@
         <v>422</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O2" s="44" t="s">
         <v>422</v>
@@ -19224,7 +19264,7 @@
         <v>427</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
@@ -19269,7 +19309,7 @@
         <v>422</v>
       </c>
       <c r="N3" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>422</v>
@@ -19587,7 +19627,7 @@
         <v>422</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>422</v>
@@ -19615,7 +19655,7 @@
         <v>427</v>
       </c>
       <c r="X7" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y7" s="4" t="s">
         <v>442</v>
@@ -19666,7 +19706,7 @@
         <v>422</v>
       </c>
       <c r="N8" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>422</v>
@@ -19694,7 +19734,7 @@
         <v>427</v>
       </c>
       <c r="X8" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y8" s="4" t="s">
         <v>446</v>
@@ -19745,7 +19785,7 @@
         <v>422</v>
       </c>
       <c r="N9" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O9" s="44" t="s">
         <v>422</v>
@@ -19775,7 +19815,7 @@
         <v>427</v>
       </c>
       <c r="X9" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y9" s="4" t="s">
         <v>451</v>
@@ -19824,7 +19864,7 @@
         <v>422</v>
       </c>
       <c r="N10" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O10" s="44" t="s">
         <v>422</v>
@@ -19854,7 +19894,7 @@
         <v>427</v>
       </c>
       <c r="X10" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y10" s="4" t="s">
         <v>305</v>
@@ -19905,7 +19945,7 @@
         <v>422</v>
       </c>
       <c r="N11" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O11" s="44" t="s">
         <v>422</v>
@@ -19935,7 +19975,7 @@
         <v>427</v>
       </c>
       <c r="X11" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y11" s="4" t="s">
         <v>305</v>
@@ -19986,7 +20026,7 @@
         <v>422</v>
       </c>
       <c r="N12" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>422</v>
@@ -20016,7 +20056,7 @@
         <v>427</v>
       </c>
       <c r="X12" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y12" s="4" t="s">
         <v>305</v>
@@ -20067,7 +20107,7 @@
         <v>422</v>
       </c>
       <c r="N13" s="169" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>422</v>
@@ -20097,7 +20137,7 @@
         <v>427</v>
       </c>
       <c r="X13" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="s">
@@ -20142,7 +20182,7 @@
         <v>422</v>
       </c>
       <c r="N14" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O14" s="44" t="s">
         <v>422</v>
@@ -20172,7 +20212,7 @@
         <v>427</v>
       </c>
       <c r="X14" s="45" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
@@ -22231,7 +22271,7 @@
       <c r="AN10" s="4"/>
       <c r="AO10" s="4"/>
     </row>
-    <row r="11" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>576</v>
       </c>
@@ -23028,7 +23068,7 @@
       <c r="AN21" s="4"/>
       <c r="AO21" s="4"/>
     </row>
-    <row r="22" spans="1:47" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>740</v>
       </c>
@@ -23115,23 +23155,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="AG21:AH21"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="AG18:AH18"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AG12:AH12"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="AG5:AH5"/>
@@ -23144,12 +23173,23 @@
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="AG20:AH20"/>
+    <mergeCell ref="AG21:AH21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{7AF2FCEE-B015-491D-BBC2-94A9F5D0C211}"/>
@@ -23420,10 +23460,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48223F2-B9CE-4371-859A-91D2188CCC8F}">
-  <dimension ref="A1:AX12"/>
+  <dimension ref="A1:AY12"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23476,9 +23516,10 @@
     <col min="47" max="47" width="20.85546875" customWidth="1"/>
     <col min="48" max="48" width="26.7109375" customWidth="1"/>
     <col min="49" max="49" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -23624,13 +23665,16 @@
         <v>24</v>
       </c>
       <c r="AW1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AX1" s="170" t="s">
         <v>1015</v>
       </c>
-      <c r="AX1" s="170" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AY1" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>653</v>
       </c>
@@ -23689,7 +23733,7 @@
       <c r="AP2" s="96"/>
       <c r="AT2" s="89"/>
     </row>
-    <row r="3" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>661</v>
       </c>
@@ -23742,7 +23786,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="4" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
         <v>664</v>
       </c>
@@ -23780,10 +23824,10 @@
         <v>655</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="Q4" s="45" t="s">
-        <v>663</v>
+        <v>782</v>
       </c>
       <c r="R4" s="98" t="s">
         <v>666</v>
@@ -23800,8 +23844,11 @@
       <c r="Z4" s="65" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AY4" s="45" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>668</v>
       </c>
@@ -23848,7 +23895,7 @@
         <v>692</v>
       </c>
       <c r="AA5" s="97" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="AB5" s="99" t="s">
         <v>91</v>
@@ -23857,13 +23904,13 @@
         <v>606</v>
       </c>
       <c r="AW5" s="65" t="s">
+        <v>1017</v>
+      </c>
+      <c r="AX5" s="65" t="s">
         <v>1018</v>
       </c>
-      <c r="AX5" s="65" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>670</v>
       </c>
@@ -23913,7 +23960,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="7" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>674</v>
       </c>
@@ -23987,7 +24034,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="65" t="s">
         <v>684</v>
       </c>
@@ -24026,6 +24073,9 @@
       </c>
       <c r="W8" s="89" t="s">
         <v>657</v>
+      </c>
+      <c r="Z8" s="45" t="s">
+        <v>660</v>
       </c>
       <c r="AA8" s="101"/>
       <c r="AF8" s="89" t="s">
@@ -24041,7 +24091,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="9" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
         <v>689</v>
       </c>
@@ -24086,7 +24136,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="10" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>693</v>
       </c>
@@ -24130,7 +24180,7 @@
         <v>695</v>
       </c>
       <c r="AM10" s="89" t="s">
-        <v>696</v>
+        <v>1022</v>
       </c>
       <c r="AN10" s="94" t="s">
         <v>697</v>
@@ -24160,7 +24210,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>700</v>
       </c>
@@ -24237,7 +24287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:50" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
         <v>705</v>
       </c>

</xml_diff>

<commit_message>
admin and api bug fixes
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestData_Api.xlsx
+++ b/Web/coyni/resources/TestData_Api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC3B64E-DBEA-4A0F-93F5-97A7B0F9F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09985221-04F9-4C2D-AC7A-BCBDC32CF867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="3495" windowWidth="10455" windowHeight="9180" firstSheet="6" activeTab="8" xr2:uid="{CB8AE841-AFC2-4DEA-A837-AD06A354DD94}"/>
+    <workbookView xWindow="4530" yWindow="4530" windowWidth="10455" windowHeight="9180" firstSheet="4" activeTab="6" xr2:uid="{CB8AE841-AFC2-4DEA-A837-AD06A354DD94}"/>
   </bookViews>
   <sheets>
     <sheet name="IdentityVerification" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5072" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5072" uniqueCount="1040">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2334,12 +2334,6 @@
     <t>Adding  Debit Card</t>
   </si>
   <si>
-    <t>testBusinenssSettingsAddSignetAccount</t>
-  </si>
-  <si>
-    <t>Add Signet Account</t>
-  </si>
-  <si>
     <t>Tolichowki</t>
   </si>
   <si>
@@ -2590,12 +2584,6 @@
   </si>
   <si>
     <t>Order Preview</t>
-  </si>
-  <si>
-    <t>tokenWalletBuyTokensSignetAccount</t>
-  </si>
-  <si>
-    <t>Buy Token - Signet Account</t>
   </si>
   <si>
     <t>SignetWallet</t>
@@ -3218,6 +3206,24 @@
   </si>
   <si>
     <t>4429 5497 8723 7628</t>
+  </si>
+  <si>
+    <t>testBusinenssSettingsAddCogentAccount</t>
+  </si>
+  <si>
+    <t>Add Cogent Account</t>
+  </si>
+  <si>
+    <t>tokenWalletBuyTokensCogentAccount</t>
+  </si>
+  <si>
+    <t>Buy Token - Cogent Account</t>
+  </si>
+  <si>
+    <t>12/07/2022</t>
+  </si>
+  <si>
+    <t>12/06/2022</t>
   </si>
 </sst>
 </file>
@@ -4662,7 +4668,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>214</v>
@@ -4677,7 +4683,7 @@
         <v>418</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J2" s="175" t="s">
         <v>215</v>
@@ -4699,13 +4705,13 @@
         <v>77</v>
       </c>
       <c r="Q2" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S2" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>79</v>
@@ -4720,7 +4726,7 @@
         <v>82</v>
       </c>
       <c r="X2" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>83</v>
@@ -4776,7 +4782,7 @@
         <v>68</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>214</v>
@@ -4791,7 +4797,7 @@
         <v>418</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J3" s="175" t="s">
         <v>215</v>
@@ -4806,16 +4812,16 @@
       </c>
       <c r="O3" s="176"/>
       <c r="P3" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="Q3" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S3" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T3" s="4" t="s">
         <v>79</v>
@@ -4830,7 +4836,7 @@
         <v>82</v>
       </c>
       <c r="X3" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y3" s="4" t="s">
         <v>83</v>
@@ -4888,7 +4894,7 @@
         <v>93</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>214</v>
@@ -4903,7 +4909,7 @@
         <v>418</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J4" s="175" t="s">
         <v>215</v>
@@ -4921,13 +4927,13 @@
         <v>94</v>
       </c>
       <c r="Q4" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S4" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>79</v>
@@ -4942,7 +4948,7 @@
         <v>82</v>
       </c>
       <c r="X4" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y4" s="4" t="s">
         <v>83</v>
@@ -5000,7 +5006,7 @@
         <v>97</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>214</v>
@@ -5015,7 +5021,7 @@
         <v>418</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J5" s="175" t="s">
         <v>215</v>
@@ -5033,13 +5039,13 @@
         <v>98</v>
       </c>
       <c r="Q5" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R5" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S5" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>79</v>
@@ -5054,7 +5060,7 @@
         <v>82</v>
       </c>
       <c r="X5" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y5" s="4" t="s">
         <v>83</v>
@@ -5112,7 +5118,7 @@
         <v>100</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>214</v>
@@ -5127,7 +5133,7 @@
         <v>418</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J6" s="175" t="s">
         <v>215</v>
@@ -5149,7 +5155,7 @@
         <v>78</v>
       </c>
       <c r="S6" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T6" s="4" t="s">
         <v>79</v>
@@ -5164,7 +5170,7 @@
         <v>82</v>
       </c>
       <c r="X6" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y6" s="4" t="s">
         <v>83</v>
@@ -5222,7 +5228,7 @@
         <v>104</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>214</v>
@@ -5237,7 +5243,7 @@
         <v>418</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J7" s="175" t="s">
         <v>215</v>
@@ -5255,13 +5261,13 @@
         <v>77</v>
       </c>
       <c r="Q7" s="177" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="R7" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S7" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T7" s="4" t="s">
         <v>79</v>
@@ -5276,7 +5282,7 @@
         <v>82</v>
       </c>
       <c r="X7" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y7" s="4" t="s">
         <v>83</v>
@@ -5334,7 +5340,7 @@
         <v>107</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>214</v>
@@ -5349,7 +5355,7 @@
         <v>418</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J8" s="175" t="s">
         <v>215</v>
@@ -5367,13 +5373,13 @@
         <v>77</v>
       </c>
       <c r="Q8" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="S8" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T8" s="4" t="s">
         <v>79</v>
@@ -5388,7 +5394,7 @@
         <v>82</v>
       </c>
       <c r="X8" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y8" s="4" t="s">
         <v>83</v>
@@ -5446,7 +5452,7 @@
         <v>111</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>214</v>
@@ -5461,7 +5467,7 @@
         <v>418</v>
       </c>
       <c r="I9" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J9" s="175" t="s">
         <v>215</v>
@@ -5479,13 +5485,13 @@
         <v>77</v>
       </c>
       <c r="Q9" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R9" s="6" t="s">
         <v>112</v>
       </c>
       <c r="S9" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T9" s="4" t="s">
         <v>79</v>
@@ -5500,7 +5506,7 @@
         <v>82</v>
       </c>
       <c r="X9" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y9" s="4" t="s">
         <v>83</v>
@@ -5558,7 +5564,7 @@
         <v>114</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>214</v>
@@ -5573,7 +5579,7 @@
         <v>418</v>
       </c>
       <c r="I10" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J10" s="175" t="s">
         <v>215</v>
@@ -5591,13 +5597,13 @@
         <v>77</v>
       </c>
       <c r="Q10" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="T10" s="4" t="s">
         <v>79</v>
@@ -5612,7 +5618,7 @@
         <v>82</v>
       </c>
       <c r="X10" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y10" s="4" t="s">
         <v>83</v>
@@ -5670,7 +5676,7 @@
         <v>118</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>214</v>
@@ -5685,7 +5691,7 @@
         <v>418</v>
       </c>
       <c r="I11" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J11" s="175" t="s">
         <v>215</v>
@@ -5703,13 +5709,13 @@
         <v>77</v>
       </c>
       <c r="Q11" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S11" s="177" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="T11" s="4" t="s">
         <v>79</v>
@@ -5724,7 +5730,7 @@
         <v>82</v>
       </c>
       <c r="X11" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y11" s="4" t="s">
         <v>83</v>
@@ -5782,7 +5788,7 @@
         <v>121</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>214</v>
@@ -5797,7 +5803,7 @@
         <v>418</v>
       </c>
       <c r="I12" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J12" s="175" t="s">
         <v>215</v>
@@ -5815,16 +5821,16 @@
         <v>77</v>
       </c>
       <c r="Q12" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R12" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S12" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>80</v>
@@ -5836,7 +5842,7 @@
         <v>82</v>
       </c>
       <c r="X12" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y12" s="4" t="s">
         <v>83</v>
@@ -5894,7 +5900,7 @@
         <v>125</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>214</v>
@@ -5909,7 +5915,7 @@
         <v>418</v>
       </c>
       <c r="I13" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J13" s="175" t="s">
         <v>215</v>
@@ -5927,13 +5933,13 @@
         <v>77</v>
       </c>
       <c r="Q13" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S13" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T13" s="4" t="s">
         <v>79</v>
@@ -5948,7 +5954,7 @@
         <v>82</v>
       </c>
       <c r="X13" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y13" s="4" t="s">
         <v>83</v>
@@ -6006,7 +6012,7 @@
         <v>130</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>214</v>
@@ -6021,7 +6027,7 @@
         <v>418</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J14" s="175" t="s">
         <v>215</v>
@@ -6039,13 +6045,13 @@
         <v>77</v>
       </c>
       <c r="Q14" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R14" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S14" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T14" s="4" t="s">
         <v>79</v>
@@ -6054,13 +6060,13 @@
         <v>80</v>
       </c>
       <c r="V14" s="177" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="W14" s="4" t="s">
         <v>82</v>
       </c>
       <c r="X14" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y14" s="4" t="s">
         <v>83</v>
@@ -6118,7 +6124,7 @@
         <v>132</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>214</v>
@@ -6133,7 +6139,7 @@
         <v>418</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J15" s="175" t="s">
         <v>215</v>
@@ -6151,13 +6157,13 @@
         <v>77</v>
       </c>
       <c r="Q15" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R15" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S15" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T15" s="4" t="s">
         <v>79</v>
@@ -6166,13 +6172,13 @@
         <v>80</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="W15" s="4" t="s">
         <v>82</v>
       </c>
       <c r="X15" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y15" s="4" t="s">
         <v>83</v>
@@ -6230,7 +6236,7 @@
         <v>135</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>214</v>
@@ -6245,7 +6251,7 @@
         <v>418</v>
       </c>
       <c r="I16" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J16" s="175" t="s">
         <v>215</v>
@@ -6263,13 +6269,13 @@
         <v>77</v>
       </c>
       <c r="Q16" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S16" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T16" s="4" t="s">
         <v>79</v>
@@ -6284,7 +6290,7 @@
         <v>82</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="Y16" s="4" t="s">
         <v>83</v>
@@ -6342,7 +6348,7 @@
         <v>139</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>214</v>
@@ -6357,7 +6363,7 @@
         <v>418</v>
       </c>
       <c r="I17" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J17" s="175" t="s">
         <v>215</v>
@@ -6375,13 +6381,13 @@
         <v>77</v>
       </c>
       <c r="Q17" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R17" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S17" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T17" s="4" t="s">
         <v>79</v>
@@ -6454,7 +6460,7 @@
         <v>143</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>214</v>
@@ -6469,7 +6475,7 @@
         <v>418</v>
       </c>
       <c r="I18" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J18" s="175" t="s">
         <v>215</v>
@@ -6487,13 +6493,13 @@
         <v>77</v>
       </c>
       <c r="Q18" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R18" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S18" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T18" s="4" t="s">
         <v>79</v>
@@ -6566,7 +6572,7 @@
         <v>146</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>214</v>
@@ -6581,7 +6587,7 @@
         <v>418</v>
       </c>
       <c r="I19" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J19" s="175" t="s">
         <v>215</v>
@@ -6599,13 +6605,13 @@
         <v>77</v>
       </c>
       <c r="Q19" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R19" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S19" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T19" s="4" t="s">
         <v>79</v>
@@ -6678,7 +6684,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>214</v>
@@ -6693,7 +6699,7 @@
         <v>418</v>
       </c>
       <c r="I20" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J20" s="175" t="s">
         <v>215</v>
@@ -6711,13 +6717,13 @@
         <v>150</v>
       </c>
       <c r="Q20" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R20" s="6" t="s">
         <v>151</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="T20" s="4" t="s">
         <v>152</v>
@@ -6784,7 +6790,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>214</v>
@@ -6799,7 +6805,7 @@
         <v>418</v>
       </c>
       <c r="I21" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J21" s="175" t="s">
         <v>215</v>
@@ -6821,13 +6827,13 @@
         <v>77</v>
       </c>
       <c r="Q21" s="177" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="R21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="S21" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T21" s="4" t="s">
         <v>79</v>
@@ -6842,7 +6848,7 @@
         <v>82</v>
       </c>
       <c r="X21" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y21" s="4" t="s">
         <v>83</v>
@@ -6898,7 +6904,7 @@
         <v>68</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>214</v>
@@ -6913,7 +6919,7 @@
         <v>418</v>
       </c>
       <c r="I22" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J22" s="175" t="s">
         <v>215</v>
@@ -6992,7 +6998,7 @@
         <v>68</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>214</v>
@@ -7007,7 +7013,7 @@
         <v>418</v>
       </c>
       <c r="I23" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J23" s="175" t="s">
         <v>215</v>
@@ -7025,7 +7031,7 @@
         <v>78</v>
       </c>
       <c r="S23" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T23" s="4" t="s">
         <v>79</v>
@@ -7040,7 +7046,7 @@
         <v>82</v>
       </c>
       <c r="X23" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y23" s="4" t="s">
         <v>83</v>
@@ -7100,7 +7106,7 @@
         <v>68</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>214</v>
@@ -7115,7 +7121,7 @@
         <v>418</v>
       </c>
       <c r="I24" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J24" s="175" t="s">
         <v>215</v>
@@ -7133,7 +7139,7 @@
         <v>78</v>
       </c>
       <c r="S24" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>79</v>
@@ -7148,7 +7154,7 @@
         <v>82</v>
       </c>
       <c r="X24" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y24" s="4" t="s">
         <v>83</v>
@@ -7212,7 +7218,7 @@
         <v>100</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>214</v>
@@ -7227,7 +7233,7 @@
         <v>418</v>
       </c>
       <c r="I25" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J25" s="175" t="s">
         <v>215</v>
@@ -7243,7 +7249,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>79</v>
@@ -7258,7 +7264,7 @@
         <v>82</v>
       </c>
       <c r="X25" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y25" s="4" t="s">
         <v>83</v>
@@ -7324,7 +7330,7 @@
         <v>146</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>214</v>
@@ -7339,7 +7345,7 @@
         <v>418</v>
       </c>
       <c r="I26" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J26" s="175" t="s">
         <v>215</v>
@@ -7357,7 +7363,7 @@
         <v>112</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T26" s="4" t="s">
         <v>79</v>
@@ -7372,7 +7378,7 @@
         <v>82</v>
       </c>
       <c r="X26" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y26" s="4" t="s">
         <v>83</v>
@@ -7438,7 +7444,7 @@
         <v>104</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>214</v>
@@ -7453,7 +7459,7 @@
         <v>418</v>
       </c>
       <c r="I27" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J27" s="175" t="s">
         <v>215</v>
@@ -7471,7 +7477,7 @@
         <v>175</v>
       </c>
       <c r="S27" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>79</v>
@@ -7486,7 +7492,7 @@
         <v>82</v>
       </c>
       <c r="X27" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y27" s="4" t="s">
         <v>83</v>
@@ -7552,7 +7558,7 @@
         <v>107</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>214</v>
@@ -7567,7 +7573,7 @@
         <v>418</v>
       </c>
       <c r="I28" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J28" s="175" t="s">
         <v>215</v>
@@ -7585,7 +7591,7 @@
         <v>177</v>
       </c>
       <c r="S28" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>79</v>
@@ -7600,7 +7606,7 @@
         <v>82</v>
       </c>
       <c r="X28" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y28" s="4" t="s">
         <v>83</v>
@@ -7666,7 +7672,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>214</v>
@@ -7681,7 +7687,7 @@
         <v>418</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J29" s="175" t="s">
         <v>215</v>
@@ -7712,7 +7718,7 @@
         <v>82</v>
       </c>
       <c r="X29" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y29" s="4" t="s">
         <v>83</v>
@@ -7778,7 +7784,7 @@
         <v>118</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>214</v>
@@ -7793,7 +7799,7 @@
         <v>418</v>
       </c>
       <c r="I30" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J30" s="175" t="s">
         <v>215</v>
@@ -7826,7 +7832,7 @@
         <v>82</v>
       </c>
       <c r="X30" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y30" s="4" t="s">
         <v>83</v>
@@ -7892,7 +7898,7 @@
         <v>121</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>214</v>
@@ -7907,7 +7913,7 @@
         <v>418</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J31" s="175" t="s">
         <v>215</v>
@@ -7925,7 +7931,7 @@
         <v>78</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T31" s="4"/>
       <c r="U31" s="4" t="s">
@@ -7938,7 +7944,7 @@
         <v>82</v>
       </c>
       <c r="X31" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y31" s="4" t="s">
         <v>83</v>
@@ -8004,7 +8010,7 @@
         <v>125</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>214</v>
@@ -8019,7 +8025,7 @@
         <v>418</v>
       </c>
       <c r="I32" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J32" s="175" t="s">
         <v>215</v>
@@ -8037,7 +8043,7 @@
         <v>78</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>79</v>
@@ -8050,7 +8056,7 @@
         <v>82</v>
       </c>
       <c r="X32" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y32" s="4" t="s">
         <v>83</v>
@@ -8116,7 +8122,7 @@
         <v>130</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>214</v>
@@ -8131,7 +8137,7 @@
         <v>418</v>
       </c>
       <c r="I33" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J33" s="175" t="s">
         <v>215</v>
@@ -8149,7 +8155,7 @@
         <v>78</v>
       </c>
       <c r="S33" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T33" s="4" t="s">
         <v>79</v>
@@ -8228,7 +8234,7 @@
         <v>132</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>214</v>
@@ -8243,7 +8249,7 @@
         <v>418</v>
       </c>
       <c r="I34" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J34" s="175" t="s">
         <v>215</v>
@@ -8261,7 +8267,7 @@
         <v>78</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T34" s="4" t="s">
         <v>79</v>
@@ -8342,7 +8348,7 @@
         <v>135</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>214</v>
@@ -8357,7 +8363,7 @@
         <v>418</v>
       </c>
       <c r="I35" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J35" s="175" t="s">
         <v>215</v>
@@ -8375,7 +8381,7 @@
         <v>78</v>
       </c>
       <c r="S35" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T35" s="4" t="s">
         <v>79</v>
@@ -8456,7 +8462,7 @@
         <v>139</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>214</v>
@@ -8471,7 +8477,7 @@
         <v>418</v>
       </c>
       <c r="I36" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J36" s="175" t="s">
         <v>215</v>
@@ -8489,7 +8495,7 @@
         <v>78</v>
       </c>
       <c r="S36" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T36" s="4" t="s">
         <v>79</v>
@@ -8504,7 +8510,7 @@
         <v>82</v>
       </c>
       <c r="X36" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y36" s="4" t="s">
         <v>83</v>
@@ -8568,7 +8574,7 @@
         <v>143</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>214</v>
@@ -8583,7 +8589,7 @@
         <v>418</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J37" s="175" t="s">
         <v>215</v>
@@ -8601,7 +8607,7 @@
         <v>78</v>
       </c>
       <c r="S37" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T37" s="4" t="s">
         <v>79</v>
@@ -8614,7 +8620,7 @@
       </c>
       <c r="W37" s="4"/>
       <c r="X37" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y37" s="4" t="s">
         <v>83</v>
@@ -8680,7 +8686,7 @@
         <v>93</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>214</v>
@@ -8695,7 +8701,7 @@
         <v>418</v>
       </c>
       <c r="I38" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J38" s="175" t="s">
         <v>215</v>
@@ -8713,7 +8719,7 @@
         <v>78</v>
       </c>
       <c r="S38" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T38" s="4" t="s">
         <v>79</v>
@@ -8728,7 +8734,7 @@
         <v>82</v>
       </c>
       <c r="X38" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y38" s="4" t="s">
         <v>83</v>
@@ -8792,7 +8798,7 @@
         <v>68</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>214</v>
@@ -8807,7 +8813,7 @@
         <v>418</v>
       </c>
       <c r="I39" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J39" s="175" t="s">
         <v>215</v>
@@ -8825,7 +8831,7 @@
         <v>151</v>
       </c>
       <c r="S39" s="175" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="T39" s="4" t="s">
         <v>152</v>
@@ -8893,7 +8899,7 @@
       <c r="BE39" s="4"/>
       <c r="BF39" s="4"/>
     </row>
-    <row r="40" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>193</v>
       </c>
@@ -8904,7 +8910,7 @@
         <v>68</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>214</v>
@@ -8919,7 +8925,7 @@
         <v>418</v>
       </c>
       <c r="I40" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J40" s="175" t="s">
         <v>215</v>
@@ -8939,7 +8945,7 @@
         <v>78</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T40" s="4" t="s">
         <v>79</v>
@@ -8954,7 +8960,7 @@
         <v>82</v>
       </c>
       <c r="X40" s="177" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="Y40" s="4" t="s">
         <v>83</v>
@@ -9009,7 +9015,7 @@
       <c r="BE40" s="4"/>
       <c r="BF40" s="4"/>
     </row>
-    <row r="41" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>194</v>
       </c>
@@ -9020,7 +9026,7 @@
         <v>68</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>214</v>
@@ -9035,7 +9041,7 @@
         <v>418</v>
       </c>
       <c r="I41" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J41" s="175" t="s">
         <v>215</v>
@@ -9132,7 +9138,7 @@
       <c r="BF41" s="4"/>
       <c r="BG41" s="4"/>
     </row>
-    <row r="42" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>212</v>
       </c>
@@ -9143,7 +9149,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>214</v>
@@ -9158,7 +9164,7 @@
         <v>418</v>
       </c>
       <c r="I42" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J42" s="175" t="s">
         <v>215</v>
@@ -9221,10 +9227,10 @@
         <v>218</v>
       </c>
       <c r="BL42" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BM42" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN42" s="17" t="s">
         <v>219</v>
@@ -9233,7 +9239,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>220</v>
       </c>
@@ -9244,7 +9250,7 @@
         <v>68</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>214</v>
@@ -9259,7 +9265,7 @@
         <v>418</v>
       </c>
       <c r="I43" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J43" s="175" t="s">
         <v>215</v>
@@ -9338,7 +9344,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>220</v>
       </c>
@@ -9349,7 +9355,7 @@
         <v>100</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>214</v>
@@ -9364,7 +9370,7 @@
         <v>418</v>
       </c>
       <c r="I44" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J44" s="175" t="s">
         <v>215</v>
@@ -9434,7 +9440,7 @@
       </c>
       <c r="BL44" s="17"/>
       <c r="BM44" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN44" s="17" t="s">
         <v>228</v>
@@ -9443,7 +9449,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>220</v>
       </c>
@@ -9454,7 +9460,7 @@
         <v>104</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>214</v>
@@ -9469,7 +9475,7 @@
         <v>418</v>
       </c>
       <c r="I45" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J45" s="175" t="s">
         <v>215</v>
@@ -9546,7 +9552,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>220</v>
       </c>
@@ -9557,7 +9563,7 @@
         <v>107</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>214</v>
@@ -9572,7 +9578,7 @@
         <v>418</v>
       </c>
       <c r="I46" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J46" s="175" t="s">
         <v>215</v>
@@ -9642,14 +9648,14 @@
         <v>231</v>
       </c>
       <c r="BM46" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN46" s="17"/>
       <c r="BO46" s="17" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>220</v>
       </c>
@@ -9660,7 +9666,7 @@
         <v>114</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>214</v>
@@ -9675,7 +9681,7 @@
         <v>418</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J47" s="175" t="s">
         <v>215</v>
@@ -9745,14 +9751,14 @@
         <v>231</v>
       </c>
       <c r="BM47" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN47" s="17" t="s">
         <v>228</v>
       </c>
       <c r="BO47" s="17"/>
     </row>
-    <row r="48" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>220</v>
       </c>
@@ -9763,7 +9769,7 @@
         <v>118</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>214</v>
@@ -9778,7 +9784,7 @@
         <v>418</v>
       </c>
       <c r="I48" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J48" s="175" t="s">
         <v>215</v>
@@ -9848,7 +9854,7 @@
         <v>231</v>
       </c>
       <c r="BM48" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN48" s="17" t="s">
         <v>228</v>
@@ -9857,7 +9863,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>220</v>
       </c>
@@ -9868,7 +9874,7 @@
         <v>121</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>214</v>
@@ -9883,7 +9889,7 @@
         <v>418</v>
       </c>
       <c r="I49" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J49" s="175" t="s">
         <v>215</v>
@@ -9953,7 +9959,7 @@
         <v>231</v>
       </c>
       <c r="BM49" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN49" s="17" t="s">
         <v>228</v>
@@ -9962,7 +9968,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>241</v>
       </c>
@@ -9973,7 +9979,7 @@
         <v>68</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>214</v>
@@ -9988,7 +9994,7 @@
         <v>418</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J50" s="175" t="s">
         <v>215</v>
@@ -10051,10 +10057,10 @@
         <v>218</v>
       </c>
       <c r="BL50" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BM50" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="BN50" s="17" t="s">
         <v>219</v>
@@ -10063,7 +10069,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="1:67" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>242</v>
       </c>
@@ -10074,7 +10080,7 @@
         <v>68</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>214</v>
@@ -10089,7 +10095,7 @@
         <v>418</v>
       </c>
       <c r="I51" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J51" s="175" t="s">
         <v>215</v>
@@ -10117,7 +10123,7 @@
         <v>68</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>214</v>
@@ -10132,7 +10138,7 @@
         <v>418</v>
       </c>
       <c r="I52" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J52" s="175" t="s">
         <v>215</v>
@@ -10162,7 +10168,7 @@
         <v>68</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>214</v>
@@ -10177,7 +10183,7 @@
         <v>418</v>
       </c>
       <c r="I53" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J53" s="175" t="s">
         <v>215</v>
@@ -10210,7 +10216,7 @@
         <v>68</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>214</v>
@@ -10225,7 +10231,7 @@
         <v>418</v>
       </c>
       <c r="I54" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J54" s="175" t="s">
         <v>215</v>
@@ -10249,7 +10255,7 @@
         <v>68</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>214</v>
@@ -10264,7 +10270,7 @@
         <v>418</v>
       </c>
       <c r="I55" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J55" s="175" t="s">
         <v>215</v>
@@ -10291,7 +10297,7 @@
         <v>68</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>214</v>
@@ -10306,7 +10312,7 @@
         <v>418</v>
       </c>
       <c r="I56" s="45" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="J56" s="175" t="s">
         <v>215</v>
@@ -10990,7 +10996,7 @@
   <dimension ref="A1:AU26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11188,7 +11194,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>745</v>
       </c>
@@ -11226,7 +11232,7 @@
         <v>686</v>
       </c>
       <c r="M2" s="70" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="N2" s="75" t="s">
         <v>688</v>
@@ -11262,12 +11268,12 @@
       <c r="Y2" s="106"/>
       <c r="AB2" s="107"/>
     </row>
-    <row r="3" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
-        <v>747</v>
+        <v>1034</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>748</v>
+        <v>1035</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>68</v>
@@ -11302,10 +11308,10 @@
       <c r="O3" s="31"/>
       <c r="P3" s="31"/>
       <c r="Q3" s="31" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="R3" s="31" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="S3" s="31" t="s">
         <v>197</v>
@@ -11319,22 +11325,22 @@
       <c r="W3" s="31"/>
       <c r="X3" s="31"/>
       <c r="Y3" s="79" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z3" s="69" t="s">
+        <v>750</v>
+      </c>
+      <c r="AA3" s="69" t="s">
         <v>751</v>
       </c>
-      <c r="Z3" s="69" t="s">
+      <c r="AG3" s="108" t="s">
         <v>752</v>
       </c>
-      <c r="AA3" s="69" t="s">
+      <c r="AH3" s="108" t="s">
         <v>753</v>
       </c>
-      <c r="AG3" s="108" t="s">
-        <v>754</v>
-      </c>
-      <c r="AH3" s="108" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>599</v>
       </c>
@@ -11378,24 +11384,24 @@
         <v>603</v>
       </c>
       <c r="AR4" s="70" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="AS4" s="70" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="AT4" s="70" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="AU4" s="70" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" ht="16.5" x14ac:dyDescent="0.3">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C5" s="70" t="s">
         <v>68</v>
@@ -11428,18 +11434,18 @@
       <c r="AE5" s="109"/>
       <c r="AF5" s="79"/>
       <c r="AO5" s="70" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="AQ5" s="79" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C6" s="70" t="s">
         <v>68</v>
@@ -11469,7 +11475,7 @@
         <v>73</v>
       </c>
       <c r="M6" s="70" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="AE6" s="109" t="s">
         <v>663</v>
@@ -11478,15 +11484,15 @@
         <v>664</v>
       </c>
       <c r="AN6" s="70" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C7" s="70" t="s">
         <v>68</v>
@@ -11519,7 +11525,7 @@
         <v>686</v>
       </c>
       <c r="M7" s="70" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="N7" s="75" t="s">
         <v>688</v>
@@ -11553,12 +11559,12 @@
       </c>
       <c r="X7" s="70"/>
     </row>
-    <row r="8" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C8" s="70" t="s">
         <v>68</v>
@@ -11588,28 +11594,28 @@
         <v>73</v>
       </c>
       <c r="L8" s="110" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="M8" s="28" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="N8" s="75" t="s">
         <v>669</v>
       </c>
       <c r="O8" s="76" t="s">
+        <v>764</v>
+      </c>
+      <c r="P8" s="77" t="s">
+        <v>765</v>
+      </c>
+      <c r="Q8" s="69" t="s">
         <v>766</v>
-      </c>
-      <c r="P8" s="77" t="s">
-        <v>767</v>
-      </c>
-      <c r="Q8" s="69" t="s">
-        <v>768</v>
       </c>
       <c r="R8" s="69" t="s">
         <v>673</v>
       </c>
       <c r="S8" s="69" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="T8" s="70" t="s">
         <v>674</v>
@@ -11630,10 +11636,10 @@
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B9" s="69" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C9" s="70" t="s">
         <v>68</v>
@@ -11666,21 +11672,21 @@
         <v>173</v>
       </c>
       <c r="AJ9" s="69" t="s">
+        <v>770</v>
+      </c>
+      <c r="AK9" s="69" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL9" s="69" t="s">
         <v>772</v>
       </c>
-      <c r="AK9" s="69" t="s">
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
         <v>773</v>
       </c>
-      <c r="AL9" s="69" t="s">
+      <c r="B10" s="111" t="s">
         <v>774</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
-        <v>775</v>
-      </c>
-      <c r="B10" s="111" t="s">
-        <v>776</v>
       </c>
       <c r="C10" s="112" t="s">
         <v>68</v>
@@ -11715,15 +11721,15 @@
       </c>
       <c r="AL10" s="109"/>
       <c r="AM10" s="70" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C11" s="112" t="s">
         <v>68</v>
@@ -11777,7 +11783,7 @@
         <v>197</v>
       </c>
       <c r="T11" s="70" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="U11" s="69" t="s">
         <v>200</v>
@@ -11794,10 +11800,10 @@
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C12" s="112" t="s">
         <v>100</v>
@@ -11863,15 +11869,15 @@
         <v>591</v>
       </c>
       <c r="X12" s="124" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C13" s="112" t="s">
         <v>104</v>
@@ -11910,7 +11916,7 @@
         <v>688</v>
       </c>
       <c r="O13" s="69" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="P13" s="121" t="s">
         <v>690</v>
@@ -11937,15 +11943,15 @@
         <v>591</v>
       </c>
       <c r="X13" s="124" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C14" s="112" t="s">
         <v>107</v>
@@ -11978,7 +11984,7 @@
         <v>686</v>
       </c>
       <c r="M14" s="125" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="N14" s="75" t="s">
         <v>688</v>
@@ -12008,15 +12014,15 @@
         <v>591</v>
       </c>
       <c r="X14" s="126" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C15" s="112" t="s">
         <v>114</v>
@@ -12058,7 +12064,7 @@
         <v>689</v>
       </c>
       <c r="P15" s="70" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="Q15" s="123" t="s">
         <v>672</v>
@@ -12082,15 +12088,15 @@
         <v>591</v>
       </c>
       <c r="X15" s="126" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="16" spans="1:47" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C16" s="112" t="s">
         <v>146</v>
@@ -12135,7 +12141,7 @@
         <v>690</v>
       </c>
       <c r="Q16" s="127" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="R16" s="123" t="s">
         <v>673</v>
@@ -12157,15 +12163,15 @@
       </c>
       <c r="X16" s="126"/>
       <c r="AP16" s="69" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C17" s="112" t="s">
         <v>118</v>
@@ -12228,15 +12234,15 @@
         <v>591</v>
       </c>
       <c r="X17" s="119" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B18" s="69" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C18" s="112" t="s">
         <v>121</v>
@@ -12299,15 +12305,15 @@
         <v>591</v>
       </c>
       <c r="X18" s="126" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C19" s="112" t="s">
         <v>125</v>
@@ -12370,15 +12376,15 @@
         <v>591</v>
       </c>
       <c r="X19" s="126" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C20" s="112" t="s">
         <v>135</v>
@@ -12443,10 +12449,10 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C21" s="112" t="s">
         <v>139</v>
@@ -12504,15 +12510,15 @@
         <v>591</v>
       </c>
       <c r="X21" s="119" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C22" s="112" t="s">
         <v>143</v>
@@ -12569,15 +12575,15 @@
         <v>591</v>
       </c>
       <c r="X22" s="119" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C23" s="112" t="s">
         <v>130</v>
@@ -12645,10 +12651,10 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C24" s="112" t="s">
         <v>132</v>
@@ -12711,15 +12717,15 @@
         <v>591</v>
       </c>
       <c r="X24" s="119" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C25" s="112" t="s">
         <v>68</v>
@@ -12749,40 +12755,40 @@
         <v>73</v>
       </c>
       <c r="L25" s="69" t="s">
+        <v>807</v>
+      </c>
+      <c r="M25" s="69" t="s">
+        <v>808</v>
+      </c>
+      <c r="O25" s="69" t="s">
         <v>809</v>
       </c>
-      <c r="M25" s="69" t="s">
+      <c r="P25" s="69" t="s">
         <v>810</v>
       </c>
-      <c r="O25" s="69" t="s">
+      <c r="Q25" s="69" t="s">
         <v>811</v>
       </c>
-      <c r="P25" s="69" t="s">
+      <c r="R25" s="69" t="s">
+        <v>811</v>
+      </c>
+      <c r="S25" s="69" t="s">
         <v>812</v>
       </c>
-      <c r="Q25" s="69" t="s">
+      <c r="U25" s="69" t="s">
         <v>813</v>
       </c>
-      <c r="R25" s="69" t="s">
-        <v>813</v>
-      </c>
-      <c r="S25" s="69" t="s">
+      <c r="W25" s="112" t="s">
         <v>814</v>
-      </c>
-      <c r="U25" s="69" t="s">
-        <v>815</v>
-      </c>
-      <c r="W25" s="112" t="s">
-        <v>816</v>
       </c>
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C26" s="112" t="s">
         <v>68</v>
@@ -12824,7 +12830,7 @@
         <v>689</v>
       </c>
       <c r="P26" s="77" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="Q26" s="69" t="s">
         <v>672</v>
@@ -12845,7 +12851,7 @@
         <v>83</v>
       </c>
       <c r="W26" s="70" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="X26" s="70"/>
     </row>
@@ -12889,7 +12895,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12960,10 +12966,10 @@
         <v>50</v>
       </c>
       <c r="M1" s="82" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="N1" s="82" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="O1" s="82" t="s">
         <v>54</v>
@@ -12975,10 +12981,10 @@
         <v>56</v>
       </c>
       <c r="R1" s="82" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="S1" s="82" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="T1" s="82" t="s">
         <v>626</v>
@@ -13002,7 +13008,7 @@
         <v>24</v>
       </c>
       <c r="AA1" s="82" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="AB1" s="82" t="s">
         <v>536</v>
@@ -13010,10 +13016,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C2" s="84" t="s">
         <v>68</v>
@@ -13043,13 +13049,13 @@
         <v>73</v>
       </c>
       <c r="L2" s="88" t="s">
+        <v>826</v>
+      </c>
+      <c r="M2" s="88" t="s">
+        <v>827</v>
+      </c>
+      <c r="N2" s="88" t="s">
         <v>828</v>
-      </c>
-      <c r="M2" s="88" t="s">
-        <v>829</v>
-      </c>
-      <c r="N2" s="88" t="s">
-        <v>830</v>
       </c>
       <c r="O2" s="129" t="s">
         <v>601</v>
@@ -13070,18 +13076,18 @@
       <c r="Y2" s="41"/>
       <c r="Z2" s="41"/>
       <c r="AA2" s="36" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="AB2" s="84" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>832</v>
+        <v>1036</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>833</v>
+        <v>1037</v>
       </c>
       <c r="C3" s="84" t="s">
         <v>68</v>
@@ -13111,25 +13117,25 @@
         <v>73</v>
       </c>
       <c r="L3" s="88" t="s">
+        <v>826</v>
+      </c>
+      <c r="M3" s="88" t="s">
+        <v>827</v>
+      </c>
+      <c r="N3" s="88" t="s">
         <v>828</v>
-      </c>
-      <c r="M3" s="88" t="s">
-        <v>829</v>
-      </c>
-      <c r="N3" s="88" t="s">
-        <v>830</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
       <c r="Q3" s="41"/>
       <c r="R3" s="88" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="S3" s="41" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="T3" s="41" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="U3" s="41" t="s">
         <v>672</v>
@@ -13141,19 +13147,19 @@
         <v>197</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="Y3" s="84" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="Z3" s="41" t="s">
         <v>83</v>
       </c>
       <c r="AA3" s="36" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="AB3" s="84" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -13231,7 +13237,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="135" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="M1" s="136" t="s">
         <v>621</v>
@@ -13249,12 +13255,12 @@
         <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C2" s="138" t="s">
         <v>68</v>
@@ -13284,18 +13290,18 @@
         <v>73</v>
       </c>
       <c r="L2" s="142" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="M2" s="55" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="137" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C3" s="138" t="s">
         <v>68</v>
@@ -13325,18 +13331,18 @@
         <v>73</v>
       </c>
       <c r="L3" s="142" t="s">
+        <v>837</v>
+      </c>
+      <c r="M3" s="55" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="137" t="s">
         <v>841</v>
       </c>
-      <c r="M3" s="55" t="s">
+      <c r="B4" s="137" t="s">
         <v>842</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="137" t="s">
-        <v>845</v>
-      </c>
-      <c r="B4" s="137" t="s">
-        <v>846</v>
       </c>
       <c r="C4" s="138" t="s">
         <v>68</v>
@@ -13366,27 +13372,27 @@
         <v>73</v>
       </c>
       <c r="L4" s="142" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="M4" s="55" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="N4" s="137" t="s">
         <v>514</v>
       </c>
       <c r="O4" s="137" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="Q4" s="138" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="137" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C5" s="138" t="s">
         <v>68</v>
@@ -13416,7 +13422,7 @@
         <v>73</v>
       </c>
       <c r="L5" s="142" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
   </sheetData>
@@ -13511,10 +13517,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B2" s="132" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C2" s="146" t="s">
         <v>68</v>
@@ -13554,7 +13560,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B3" s="69" t="s">
         <v>500</v>
@@ -13598,7 +13604,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B4" s="69" t="s">
         <v>500</v>
@@ -13642,7 +13648,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B5" s="69" t="s">
         <v>501</v>
@@ -13686,7 +13692,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>503</v>
@@ -13730,7 +13736,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B7" s="69" t="s">
         <v>503</v>
@@ -13774,7 +13780,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B8" s="69" t="s">
         <v>503</v>
@@ -13818,7 +13824,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B9" s="69" t="s">
         <v>503</v>
@@ -13862,7 +13868,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>508</v>
@@ -13898,15 +13904,15 @@
         <v>265</v>
       </c>
       <c r="N10" s="149" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C11" s="146" t="s">
         <v>68</v>
@@ -13936,7 +13942,7 @@
         <v>73</v>
       </c>
       <c r="M11" s="69" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="N11" s="69" t="s">
         <v>119</v>
@@ -13947,10 +13953,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="69" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C12" s="146" t="s">
         <v>100</v>
@@ -13980,7 +13986,7 @@
         <v>73</v>
       </c>
       <c r="M12" s="69" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="N12" s="69" t="s">
         <v>119</v>
@@ -13991,10 +13997,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C13" s="146" t="s">
         <v>104</v>
@@ -14024,7 +14030,7 @@
         <v>73</v>
       </c>
       <c r="M13" s="69" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="N13" s="69" t="s">
         <v>119</v>
@@ -14035,10 +14041,10 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="69" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C14" s="146" t="s">
         <v>107</v>
@@ -14068,7 +14074,7 @@
         <v>73</v>
       </c>
       <c r="M14" s="69" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="N14" s="69" t="s">
         <v>119</v>
@@ -14079,10 +14085,10 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="69" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C15" s="146" t="s">
         <v>114</v>
@@ -14239,18 +14245,18 @@
         <v>50</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14287,13 +14293,13 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="11" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -14378,7 +14384,7 @@
         <v>50</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>41</v>
@@ -14387,16 +14393,16 @@
         <v>42</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>267</v>
@@ -14408,24 +14414,24 @@
         <v>11</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B2" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14455,15 +14461,15 @@
         <v>73</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B3" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>68</v>
@@ -14493,51 +14499,51 @@
         <v>73</v>
       </c>
       <c r="M3" s="11" t="s">
+        <v>879</v>
+      </c>
+      <c r="N3" t="s">
+        <v>880</v>
+      </c>
+      <c r="O3" t="s">
+        <v>881</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>882</v>
+      </c>
+      <c r="Q3" s="17" t="s">
         <v>883</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" s="131" t="s">
         <v>884</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" s="153" t="s">
         <v>885</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>886</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>887</v>
-      </c>
-      <c r="R3" s="131" t="s">
-        <v>888</v>
-      </c>
-      <c r="S3" s="153" t="s">
-        <v>889</v>
-      </c>
       <c r="T3" s="153" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="U3" t="s">
         <v>514</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="W3" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="Z3" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="B4" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>68</v>
@@ -14570,10 +14576,10 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="B5" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>68</v>
@@ -14608,10 +14614,10 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="B6" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>100</v>
@@ -14641,15 +14647,15 @@
         <v>73</v>
       </c>
       <c r="X6" s="155" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>892</v>
+      </c>
+      <c r="B7" t="s">
         <v>896</v>
-      </c>
-      <c r="B7" t="s">
-        <v>900</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>104</v>
@@ -14679,15 +14685,15 @@
         <v>73</v>
       </c>
       <c r="X7" s="154" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="B8" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>68</v>
@@ -14719,10 +14725,10 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B9" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>68</v>
@@ -14755,10 +14761,10 @@
         <v>514</v>
       </c>
       <c r="V9" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="Y9" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -14842,10 +14848,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="B2" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -14875,7 +14881,7 @@
         <v>73</v>
       </c>
       <c r="L2" s="156" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -14965,10 +14971,10 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B2" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C2" s="143" t="s">
         <v>68</v>
@@ -15008,7 +15014,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B3" t="s">
         <v>500</v>
@@ -15052,7 +15058,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B4" t="s">
         <v>501</v>
@@ -15096,7 +15102,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B5" t="s">
         <v>503</v>
@@ -15140,7 +15146,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B6" t="s">
         <v>503</v>
@@ -15184,7 +15190,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B7" t="s">
         <v>503</v>
@@ -15228,7 +15234,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B8" t="s">
         <v>503</v>
@@ -15272,10 +15278,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B9" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C9" s="143" t="s">
         <v>125</v>
@@ -15305,7 +15311,7 @@
         <v>73</v>
       </c>
       <c r="M9" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="N9" t="s">
         <v>119</v>
@@ -15316,10 +15322,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B10" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C10" s="143" t="s">
         <v>130</v>
@@ -15349,7 +15355,7 @@
         <v>73</v>
       </c>
       <c r="M10" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="N10" t="s">
         <v>119</v>
@@ -15360,10 +15366,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B11" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C11" s="143" t="s">
         <v>132</v>
@@ -15393,7 +15399,7 @@
         <v>73</v>
       </c>
       <c r="M11" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="N11" t="s">
         <v>119</v>
@@ -15402,12 +15408,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="B12" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="C12" s="143" t="s">
         <v>68</v>
@@ -15526,21 +15532,21 @@
         <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -15567,16 +15573,16 @@
         <v>215</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -16280,10 +16286,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="B2" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16313,15 +16319,15 @@
         <v>73</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="B3" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16351,15 +16357,15 @@
         <v>73</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="B4" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>68</v>
@@ -16389,7 +16395,7 @@
         <v>73</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -16467,15 +16473,15 @@
         <v>50</v>
       </c>
       <c r="M1" s="152" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="B2" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16505,10 +16511,10 @@
         <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="M2" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
     </row>
   </sheetData>
@@ -16584,10 +16590,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="B2" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16617,15 +16623,15 @@
         <v>73</v>
       </c>
       <c r="L2" s="45" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="B3" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16655,7 +16661,7 @@
         <v>73</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
   </sheetData>
@@ -16735,13 +16741,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="152" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="M1" s="152" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="N1" s="152" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="O1" s="152" t="s">
         <v>627</v>
@@ -16759,15 +16765,15 @@
         <v>51</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -16797,30 +16803,30 @@
         <v>73</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="P2" s="157"/>
       <c r="Q2" s="157"/>
       <c r="R2" s="157"/>
       <c r="T2" s="158" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>68</v>
@@ -16850,25 +16856,25 @@
         <v>73</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="M3" s="157"/>
       <c r="N3" s="33"/>
       <c r="O3" s="157"/>
       <c r="P3" s="159" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="Q3" s="159" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="R3" s="157"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>68</v>
@@ -16900,22 +16906,22 @@
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
       <c r="N4" s="9" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="O4" s="157"/>
       <c r="P4" s="159"/>
       <c r="Q4" s="159"/>
       <c r="R4" s="157" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="S4" s="160"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="99" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>68</v>
@@ -16945,16 +16951,16 @@
         <v>73</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -17037,10 +17043,10 @@
         <v>50</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>468</v>
@@ -17051,10 +17057,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="B2" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>68</v>
@@ -17084,15 +17090,15 @@
         <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="B3" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>68</v>
@@ -17122,19 +17128,19 @@
         <v>73</v>
       </c>
       <c r="L3" t="s">
+        <v>960</v>
+      </c>
+      <c r="M3" t="s">
+        <v>963</v>
+      </c>
+      <c r="N3" t="s">
         <v>964</v>
-      </c>
-      <c r="M3" t="s">
-        <v>967</v>
-      </c>
-      <c r="N3" t="s">
-        <v>968</v>
       </c>
       <c r="O3" t="s">
         <v>514</v>
       </c>
       <c r="P3" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -17206,15 +17212,15 @@
         <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="B2" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>68</v>
@@ -17244,7 +17250,7 @@
         <v>73</v>
       </c>
       <c r="L2" s="48" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
   </sheetData>
@@ -17316,21 +17322,21 @@
         <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>68</v>
@@ -17357,16 +17363,16 @@
         <v>215</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
   </sheetData>
@@ -17445,39 +17451,39 @@
         <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>517</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="C2" s="162" t="s">
         <v>68</v>
@@ -17507,15 +17513,15 @@
         <v>73</v>
       </c>
       <c r="S2" s="165" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="C3" s="162" t="s">
         <v>68</v>
@@ -17545,33 +17551,33 @@
         <v>73</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="M3" s="165" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="N3" s="165" t="s">
         <v>28</v>
       </c>
       <c r="O3" s="165" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="P3" s="165" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="R3" s="162" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="B4" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="C4" s="162" t="s">
         <v>68</v>
@@ -17601,7 +17607,7 @@
         <v>73</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>
@@ -18871,7 +18877,7 @@
       <c r="Q11" s="33"/>
       <c r="R11" s="33"/>
       <c r="S11" s="45" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="T11" s="33" t="s">
         <v>90</v>
@@ -18882,7 +18888,7 @@
       <c r="V11" s="41"/>
       <c r="W11" s="41"/>
       <c r="X11" s="45" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -19249,7 +19255,7 @@
         <v>413</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O2" s="44" t="s">
         <v>413</v>
@@ -19279,7 +19285,7 @@
         <v>418</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
@@ -19324,7 +19330,7 @@
         <v>413</v>
       </c>
       <c r="N3" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>413</v>
@@ -19642,7 +19648,7 @@
         <v>413</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>413</v>
@@ -19670,7 +19676,7 @@
         <v>418</v>
       </c>
       <c r="X7" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y7" s="4" t="s">
         <v>433</v>
@@ -19721,7 +19727,7 @@
         <v>413</v>
       </c>
       <c r="N8" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>413</v>
@@ -19749,7 +19755,7 @@
         <v>418</v>
       </c>
       <c r="X8" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y8" s="4" t="s">
         <v>437</v>
@@ -19800,7 +19806,7 @@
         <v>413</v>
       </c>
       <c r="N9" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O9" s="44" t="s">
         <v>413</v>
@@ -19830,7 +19836,7 @@
         <v>418</v>
       </c>
       <c r="X9" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y9" s="4" t="s">
         <v>442</v>
@@ -19879,7 +19885,7 @@
         <v>413</v>
       </c>
       <c r="N10" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O10" s="44" t="s">
         <v>413</v>
@@ -19909,7 +19915,7 @@
         <v>418</v>
       </c>
       <c r="X10" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y10" s="4" t="s">
         <v>296</v>
@@ -19960,7 +19966,7 @@
         <v>413</v>
       </c>
       <c r="N11" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O11" s="44" t="s">
         <v>413</v>
@@ -19990,7 +19996,7 @@
         <v>418</v>
       </c>
       <c r="X11" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y11" s="4" t="s">
         <v>296</v>
@@ -20041,7 +20047,7 @@
         <v>413</v>
       </c>
       <c r="N12" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>413</v>
@@ -20071,7 +20077,7 @@
         <v>418</v>
       </c>
       <c r="X12" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y12" s="4" t="s">
         <v>296</v>
@@ -20122,7 +20128,7 @@
         <v>413</v>
       </c>
       <c r="N13" s="169" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>413</v>
@@ -20152,7 +20158,7 @@
         <v>418</v>
       </c>
       <c r="X13" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="s">
@@ -20197,7 +20203,7 @@
         <v>413</v>
       </c>
       <c r="N14" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O14" s="44" t="s">
         <v>413</v>
@@ -20227,7 +20233,7 @@
         <v>418</v>
       </c>
       <c r="X14" s="45" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
@@ -21387,9 +21393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70794812-CAF1-423A-BCF8-A14AAF051BEB}">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS22" sqref="AS22"/>
+      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21769,10 +21775,10 @@
         <v>379</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>547</v>
+        <v>1039</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>548</v>
+        <v>1038</v>
       </c>
       <c r="W4" s="59" t="s">
         <v>547</v>
@@ -22286,7 +22292,7 @@
       <c r="AN10" s="4"/>
       <c r="AO10" s="4"/>
     </row>
-    <row r="11" spans="1:47" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>567</v>
       </c>
@@ -23083,7 +23089,7 @@
       <c r="AN21" s="4"/>
       <c r="AO21" s="4"/>
     </row>
-    <row r="22" spans="1:47" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>731</v>
       </c>
@@ -23156,26 +23162,37 @@
         <v>218</v>
       </c>
       <c r="AR22" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="AS22" s="17" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="AT22" s="17" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="AU22" s="17" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="AG20:AH20"/>
+    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="AG15:AH15"/>
     <mergeCell ref="AG12:AH12"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="AG5:AH5"/>
@@ -23188,23 +23205,12 @@
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="AG18:AH18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="AG4:AH4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{7AF2FCEE-B015-491D-BBC2-94A9F5D0C211}"/>
@@ -23477,8 +23483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48223F2-B9CE-4371-859A-91D2188CCC8F}">
   <dimension ref="A1:AY12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AM10" sqref="AM10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23680,13 +23686,13 @@
         <v>24</v>
       </c>
       <c r="AW1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="AX1" s="170" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="AY1" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="2" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -23839,7 +23845,7 @@
         <v>646</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="Q4" s="78" t="s">
         <v>654</v>
@@ -23910,7 +23916,7 @@
         <v>683</v>
       </c>
       <c r="AA5" s="97" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="AB5" s="99" t="s">
         <v>90</v>
@@ -23919,10 +23925,10 @@
         <v>597</v>
       </c>
       <c r="AW5" s="65" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="AX5" s="65" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="6" spans="1:51" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -24192,31 +24198,31 @@
         <v>678</v>
       </c>
       <c r="AL10" s="91" t="s">
+        <v>1029</v>
+      </c>
+      <c r="AM10" s="89" t="s">
         <v>1033</v>
-      </c>
-      <c r="AM10" s="89" t="s">
-        <v>1037</v>
       </c>
       <c r="AN10" s="65" t="s">
         <v>669</v>
       </c>
       <c r="AO10" s="95" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="AP10" s="96" t="s">
+        <v>1027</v>
+      </c>
+      <c r="AQ10" s="65" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AR10" s="65" t="s">
         <v>1031</v>
-      </c>
-      <c r="AQ10" s="65" t="s">
-        <v>1034</v>
-      </c>
-      <c r="AR10" s="65" t="s">
-        <v>1035</v>
       </c>
       <c r="AS10" s="65" t="s">
         <v>197</v>
       </c>
       <c r="AT10" s="89" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="AU10" s="65" t="s">
         <v>200</v>

</xml_diff>